<commit_message>
Aggiunta tasto Aggiungi Collaboratore, con relativa create
</commit_message>
<xml_diff>
--- a/App_Progetto/App_Progetto/DatiDb/dati.xlsx
+++ b/App_Progetto/App_Progetto/DatiDb/dati.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="72" windowWidth="10536" windowHeight="8700"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="10536" windowHeight="8700" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Utente" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,13 @@
     <sheet name="Sensore" sheetId="6" r:id="rId5"/>
     <sheet name="Misuarazione" sheetId="7" r:id="rId6"/>
     <sheet name="Piano" sheetId="10" r:id="rId7"/>
-    <sheet name="Piano_Veccio" sheetId="8" r:id="rId8"/>
-    <sheet name="Condizione" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="132">
   <si>
     <t>userName</t>
   </si>
@@ -96,24 +94,9 @@
     <t>codice_attuatore</t>
   </si>
   <si>
-    <t>tipo_attuatore</t>
-  </si>
-  <si>
-    <t>stato</t>
-  </si>
-  <si>
-    <t>foglio_terreno</t>
-  </si>
-  <si>
     <t>codice_sensore</t>
   </si>
   <si>
-    <t>stato_sensore</t>
-  </si>
-  <si>
-    <t>tipo_sensore</t>
-  </si>
-  <si>
     <t>Umidità</t>
   </si>
   <si>
@@ -123,21 +106,9 @@
     <t>Luminosità</t>
   </si>
   <si>
-    <t>data_misurazione</t>
-  </si>
-  <si>
     <t>cod_sensore</t>
   </si>
   <si>
-    <t>valore</t>
-  </si>
-  <si>
-    <t>tipo_misurazione</t>
-  </si>
-  <si>
-    <t>ora_misurazione</t>
-  </si>
-  <si>
     <t>gradi</t>
   </si>
   <si>
@@ -147,33 +118,6 @@
     <t>lux</t>
   </si>
   <si>
-    <t>codice_piano</t>
-  </si>
-  <si>
-    <t>orario_attivaz</t>
-  </si>
-  <si>
-    <t>orario_disattivaz</t>
-  </si>
-  <si>
-    <t>orario_att_default</t>
-  </si>
-  <si>
-    <t>orario_disatt_default</t>
-  </si>
-  <si>
-    <t>cod_att</t>
-  </si>
-  <si>
-    <t>cod_piano</t>
-  </si>
-  <si>
-    <t>attivazione</t>
-  </si>
-  <si>
-    <t>disattivazione</t>
-  </si>
-  <si>
     <t>umidità &lt; 12</t>
   </si>
   <si>
@@ -297,21 +241,9 @@
     <t>SEN155</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>id_terr</t>
-  </si>
-  <si>
-    <t>id_terreno</t>
-  </si>
-  <si>
     <t>CodiceSensore</t>
   </si>
   <si>
-    <t>SensoreId</t>
-  </si>
-  <si>
     <t>20029298@studenti.uniupo.it</t>
   </si>
   <si>
@@ -412,6 +344,78 @@
   </si>
   <si>
     <t>a361ae80-89bd-44b6-abbe-83390e3cbb98</t>
+  </si>
+  <si>
+    <t>alessandro.suardi@hotmail.com</t>
+  </si>
+  <si>
+    <t>Alessandro123@</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Agricoltore, Collaboratore</t>
+  </si>
+  <si>
+    <t>e3cf0247-e837-47b6-8d4b-7e31914c4082</t>
+  </si>
+  <si>
+    <t>e3cf0247-e837-47b6-8d4b-7e31914c4083</t>
+  </si>
+  <si>
+    <t>e3cf0247-e837-47b6-8d4b-7e31914c4084</t>
+  </si>
+  <si>
+    <t>TipoAttuatore</t>
+  </si>
+  <si>
+    <t>Standby</t>
+  </si>
+  <si>
+    <t>Attivazione</t>
+  </si>
+  <si>
+    <t>StatoSensore</t>
+  </si>
+  <si>
+    <t>TipoSensore</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Ora</t>
+  </si>
+  <si>
+    <t>DataOra</t>
+  </si>
+  <si>
+    <t>Valore</t>
+  </si>
+  <si>
+    <t>TipoMisurazione</t>
+  </si>
+  <si>
+    <t>CodicePiano</t>
+  </si>
+  <si>
+    <t>CodAtt</t>
+  </si>
+  <si>
+    <t>OrarioAttivazione</t>
+  </si>
+  <si>
+    <t>OrarioDisattivazione</t>
+  </si>
+  <si>
+    <t>OrarioAttDefault</t>
+  </si>
+  <si>
+    <t>OrarioDisattDefault</t>
+  </si>
+  <si>
+    <t>CondAttivazione</t>
+  </si>
+  <si>
+    <t>CondDisattivazione</t>
   </si>
 </sst>
 </file>
@@ -813,15 +817,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="36.44140625" customWidth="1"/>
     <col min="2" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -845,21 +849,21 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="24.75" customHeight="1">
       <c r="A3" s="15" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -869,29 +873,29 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="7" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="24.75" customHeight="1">
       <c r="A4" s="15" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="7" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="24.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -900,47 +904,53 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="24.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="24.75" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A8" s="2"/>
+      <c r="A8" s="15" t="s">
+        <v>108</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="24.75" customHeight="1">
@@ -989,9 +999,11 @@
     <hyperlink ref="A5" r:id="rId3"/>
     <hyperlink ref="A6" r:id="rId4"/>
     <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1000,7 +1012,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J13" sqref="J13:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1013,25 +1025,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1054,7 +1066,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="16"/>
@@ -1079,7 +1091,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="16"/>
@@ -1104,9 +1116,10 @@
         <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I4" s="17"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
@@ -1128,7 +1141,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="16"/>
@@ -1153,7 +1166,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="16"/>
@@ -1178,9 +1191,9 @@
         <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I7" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
@@ -1202,7 +1215,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="16"/>
@@ -1227,9 +1240,9 @@
         <v>17</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I9" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="I9" s="17"/>
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10">
@@ -1252,7 +1265,7 @@
         <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="16"/>
@@ -1277,9 +1290,9 @@
         <v>19</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I11" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="I11" s="17"/>
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10">
@@ -1302,9 +1315,9 @@
         <v>21</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I12" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="I12" s="17"/>
       <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:10">
@@ -1324,12 +1337,13 @@
         <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="I13" s="17"/>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
@@ -1351,9 +1365,10 @@
         <v>17</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I14" s="17"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
@@ -1375,7 +1390,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I15" s="18"/>
       <c r="J15" s="16"/>
@@ -1400,7 +1415,7 @@
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I16" s="19"/>
     </row>
@@ -1412,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1427,16 +1442,16 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1444,16 +1459,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1461,16 +1476,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1478,16 +1493,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1495,16 +1510,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1512,16 +1527,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1529,16 +1544,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1546,16 +1561,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1563,16 +1578,16 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D9">
         <v>17</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1580,16 +1595,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1597,16 +1612,16 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1614,16 +1629,16 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D12">
         <v>9</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1631,16 +1646,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D13">
         <v>14</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1648,16 +1663,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D14">
         <v>7</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1665,16 +1680,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1682,16 +1697,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D16">
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1699,16 +1714,16 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D17">
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1716,16 +1731,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1733,16 +1748,16 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D19">
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1750,16 +1765,16 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D20">
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1767,16 +1782,16 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D21">
         <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1784,16 +1799,16 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D22">
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1801,16 +1816,135 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D23">
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>103</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1831,13 +1965,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
@@ -1848,30 +1983,30 @@
         <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1887,13 +2022,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1909,13 +2044,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1931,13 +2066,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1953,13 +2088,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1975,13 +2110,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1997,13 +2132,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2019,13 +2154,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2041,13 +2176,13 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2063,13 +2198,13 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2085,13 +2220,13 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2107,13 +2242,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2129,13 +2264,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -2151,13 +2286,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2180,46 +2315,44 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -2228,20 +2361,17 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2">
         <v>6</v>
       </c>
-      <c r="F2" s="2">
-        <v>22</v>
-      </c>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -2250,20 +2380,17 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
-        <v>45</v>
-      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -2272,20 +2399,17 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2">
         <v>3</v>
       </c>
-      <c r="F4" s="2">
-        <v>2</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -2294,20 +2418,17 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="2">
-        <v>45</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -2316,20 +2437,17 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="2">
-        <v>44</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -2338,20 +2456,17 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>14</v>
       </c>
-      <c r="F7" s="2">
-        <v>46</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -2360,20 +2475,17 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2">
         <v>13</v>
       </c>
-      <c r="F8" s="2">
-        <v>3</v>
-      </c>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -2382,20 +2494,17 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
         <v>13</v>
       </c>
-      <c r="F9" s="2">
-        <v>3</v>
-      </c>
+      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -2404,20 +2513,17 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2">
         <v>12</v>
       </c>
-      <c r="F10" s="2">
-        <v>2</v>
-      </c>
+      <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -2426,20 +2532,17 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2">
         <v>11</v>
       </c>
-      <c r="F11" s="2">
-        <v>57</v>
-      </c>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -2448,20 +2551,17 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
-      <c r="F12" s="2">
-        <v>12</v>
-      </c>
+      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -2470,20 +2570,17 @@
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2">
         <v>9</v>
       </c>
-      <c r="F13" s="2">
-        <v>2</v>
-      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -2492,20 +2589,17 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2">
         <v>8</v>
       </c>
-      <c r="F14" s="2">
-        <v>55</v>
-      </c>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -2514,18 +2608,15 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2">
         <v>7</v>
       </c>
-      <c r="F15" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -2534,13 +2625,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E16" s="2">
         <v>5</v>
-      </c>
-      <c r="F16" s="2">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2553,47 +2641,46 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="16.88671875" customWidth="1"/>
+    <col min="1" max="2" width="16.88671875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" customWidth="1"/>
     <col min="6" max="6" width="12.109375" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="11">
         <v>44875</v>
       </c>
@@ -2604,7 +2691,7 @@
         <v>44875.666666666664</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -2613,11 +2700,10 @@
         <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="12">
         <v>44882</v>
       </c>
@@ -2628,7 +2714,7 @@
         <v>44882.75</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E3" s="2">
         <v>6</v>
@@ -2637,11 +2723,10 @@
         <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="12">
         <v>44881</v>
       </c>
@@ -2652,7 +2737,7 @@
         <v>44881.543194444443</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E4" s="2">
         <v>6</v>
@@ -2661,11 +2746,10 @@
         <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="13">
         <v>44876</v>
       </c>
@@ -2676,7 +2760,7 @@
         <v>44876.656388888892</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2">
         <v>7</v>
@@ -2685,11 +2769,10 @@
         <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="13">
         <v>44866</v>
       </c>
@@ -2700,7 +2783,7 @@
         <v>44866.698055555556</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2">
         <v>7</v>
@@ -2709,11 +2792,10 @@
         <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="12">
         <v>44883</v>
       </c>
@@ -2724,7 +2806,7 @@
         <v>44883.625</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="E7" s="2">
         <v>3</v>
@@ -2733,11 +2815,10 @@
         <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="12">
         <v>44867</v>
       </c>
@@ -2748,7 +2829,7 @@
         <v>44867.584861111114</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="E8" s="2">
         <v>3</v>
@@ -2757,11 +2838,10 @@
         <v>78</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="12">
         <v>44877</v>
       </c>
@@ -2772,7 +2852,7 @@
         <v>44877.668194444443</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2">
         <v>9</v>
@@ -2781,11 +2861,10 @@
         <v>45</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="12">
         <v>44886</v>
       </c>
@@ -2796,7 +2875,7 @@
         <v>44886.583333333336</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="E10" s="2">
         <v>4</v>
@@ -2805,11 +2884,10 @@
         <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="12">
         <v>44874</v>
       </c>
@@ -2820,7 +2898,7 @@
         <v>44874.626527777778</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="E11" s="2">
         <v>13</v>
@@ -2829,11 +2907,10 @@
         <v>21</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="12">
         <v>44876</v>
       </c>
@@ -2844,7 +2921,7 @@
         <v>44876.501527777778</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -2853,11 +2930,10 @@
         <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="13">
         <v>44867</v>
       </c>
@@ -2868,7 +2944,7 @@
         <v>44867.383483796293</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2">
         <v>8</v>
@@ -2877,11 +2953,10 @@
         <v>18</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="13">
         <v>44875</v>
       </c>
@@ -2892,7 +2967,7 @@
         <v>44875.523032407407</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E14" s="2">
         <v>8</v>
@@ -2901,11 +2976,10 @@
         <v>20</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="13">
         <v>44856</v>
       </c>
@@ -2916,7 +2990,7 @@
         <v>44856.583969907406</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E15" s="2">
         <v>14</v>
@@ -2925,10 +2999,10 @@
         <v>22</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="13">
         <v>44885</v>
       </c>
@@ -2939,7 +3013,7 @@
         <v>44885.5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E16" s="2">
         <v>5</v>
@@ -2948,7 +3022,7 @@
         <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2962,7 +3036,7 @@
         <v>44874.583333333336</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E17" s="2">
         <v>5</v>
@@ -2971,7 +3045,7 @@
         <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2985,7 +3059,7 @@
         <v>44885.541666666664</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E18" s="2">
         <v>11</v>
@@ -2994,7 +3068,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3008,7 +3082,7 @@
         <v>44878.709861111114</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E19" s="2">
         <v>10</v>
@@ -3017,7 +3091,7 @@
         <v>21</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3031,7 +3105,7 @@
         <v>44879.708333333336</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="E20" s="2">
         <v>15</v>
@@ -3040,7 +3114,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3054,7 +3128,7 @@
         <v>44880.75</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="E21" s="10">
         <v>12</v>
@@ -3063,7 +3137,7 @@
         <v>45</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3117,10 +3191,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3130,36 +3204,37 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="7" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>130</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3176,19 +3251,16 @@
         <v>0.75</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3205,19 +3277,16 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="H3" s="2">
         <v>10</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3234,19 +3303,16 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2">
         <v>2</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3263,19 +3329,16 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="H5" s="2">
         <v>3</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3292,19 +3355,16 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H6" s="2">
         <v>4</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3321,19 +3381,16 @@
         <v>0.75</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H7" s="2">
         <v>5</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3350,19 +3407,16 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="H8" s="2">
         <v>14</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3379,19 +3433,16 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="H9" s="2">
         <v>6</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3408,19 +3459,16 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H10" s="2">
         <v>7</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3437,19 +3485,16 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="H11" s="2">
         <v>9</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3466,19 +3511,16 @@
         <v>0.75</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="H12" s="2">
         <v>8</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3495,19 +3537,16 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="H13" s="2">
         <v>12</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3524,19 +3563,16 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="H14" s="2">
         <v>11</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3553,16 +3589,13 @@
         <v>0.6875</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="H15" s="2">
         <v>13</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3571,511 +3604,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.6875</v>
-      </c>
-      <c r="D3" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.77083333333333304</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.6875</v>
-      </c>
-      <c r="D7" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0.6875</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="D11" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0.6875</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1.6041666666666665</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0.6875</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>